<commit_message>
add new data hold a cup. implementing svm to data. need to label data.
</commit_message>
<xml_diff>
--- a/hand_jupyter_notebook/Rescaled_EMG_time.xlsx
+++ b/hand_jupyter_notebook/Rescaled_EMG_time.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thang Le\Documents\Python Scripts\Hand_Jupyter_notebook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thang Le\Documents\github\smart_pros\hand_jupyter_notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1465140-207B-492A-99AB-2C5C86088B11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3D73B9-96D7-4651-A6AC-3450CDC89AF9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{05AF3264-AA5A-A04B-874A-A70609F1B997}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="7" xr2:uid="{05AF3264-AA5A-A04B-874A-A70609F1B997}"/>
   </bookViews>
   <sheets>
     <sheet name="Rest 1" sheetId="1" r:id="rId1"/>
     <sheet name="muscle_1" sheetId="2" r:id="rId2"/>
     <sheet name="Rest 2" sheetId="3" r:id="rId3"/>
-    <sheet name="muscle 2" sheetId="4" r:id="rId4"/>
+    <sheet name="muscle_2" sheetId="4" r:id="rId4"/>
     <sheet name="Rest 3" sheetId="5" r:id="rId5"/>
-    <sheet name="muscle 3" sheetId="6" r:id="rId6"/>
-    <sheet name="rest 4" sheetId="7" r:id="rId7"/>
-    <sheet name="muscle 4" sheetId="8" r:id="rId8"/>
+    <sheet name="muscle_3" sheetId="6" r:id="rId6"/>
+    <sheet name="rest_4" sheetId="7" r:id="rId7"/>
+    <sheet name="muscle_4" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="2395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2415" uniqueCount="2395">
   <si>
     <t>15:14:23.297 -&gt; 3010</t>
   </si>
@@ -7391,16 +7391,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>511175</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>625475</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7429,8 +7429,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1320800" y="1460500"/>
-          <a:ext cx="10058400" cy="7543800"/>
+          <a:off x="3692525" y="1352550"/>
+          <a:ext cx="10058400" cy="7429500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11415,7 +11415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9685408-9F45-7E4A-80C0-FD540EF85A27}">
   <dimension ref="A1:C300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -15033,7 +15033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526634A0-5261-8342-A150-3B2396035B33}">
   <dimension ref="A1:C300"/>
   <sheetViews>
-    <sheetView topLeftCell="A288" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -18651,12 +18651,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544D9103-AD09-524F-9A85-FEC92ABF5EB9}">
   <dimension ref="A1:C300"/>
   <sheetViews>
-    <sheetView topLeftCell="A281" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
   <cols>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
@@ -25888,7 +25889,7 @@
   <dimension ref="A1:C300"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
@@ -31920,2412 +31921,3615 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B42CD52-747F-C64E-9D93-8CC3540F35B3}">
-  <dimension ref="A1:B300"/>
+  <dimension ref="A1:C300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <cols>
+    <col min="1" max="1" width="19.875" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A1" t="s">
         <v>299</v>
       </c>
       <c r="B1" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C1" t="s">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A2" t="s">
         <v>2095</v>
       </c>
       <c r="B2">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C2">
+        <f>RIGHT(A2,4)-RIGHT($A$2,4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A3" t="s">
         <v>2096</v>
       </c>
       <c r="B3">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C3">
+        <f t="shared" ref="C3:C66" si="0">RIGHT(A3,4)-RIGHT($A$2,4)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A4" t="s">
         <v>2097</v>
       </c>
       <c r="B4">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A5" t="s">
         <v>2098</v>
       </c>
       <c r="B5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A6" t="s">
         <v>2099</v>
       </c>
       <c r="B6">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A7" t="s">
         <v>2100</v>
       </c>
       <c r="B7">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A8" t="s">
         <v>2101</v>
       </c>
       <c r="B8">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A9" t="s">
         <v>2102</v>
       </c>
       <c r="B9">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A10" t="s">
         <v>2103</v>
       </c>
       <c r="B10">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A11" t="s">
         <v>2104</v>
       </c>
       <c r="B11">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A12" t="s">
         <v>2105</v>
       </c>
       <c r="B12">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A13" t="s">
         <v>2106</v>
       </c>
       <c r="B13">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A14" t="s">
         <v>2107</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A15" t="s">
         <v>2108</v>
       </c>
       <c r="B15">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A16" t="s">
         <v>2109</v>
       </c>
       <c r="B16">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A17" t="s">
         <v>2110</v>
       </c>
       <c r="B17">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A18" t="s">
         <v>2111</v>
       </c>
       <c r="B18">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A19" t="s">
         <v>2112</v>
       </c>
       <c r="B19">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A20" t="s">
         <v>2113</v>
       </c>
       <c r="B20">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A21" t="s">
         <v>2114</v>
       </c>
       <c r="B21">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A22" t="s">
         <v>2115</v>
       </c>
       <c r="B22">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A23" t="s">
         <v>2116</v>
       </c>
       <c r="B23">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A24" t="s">
         <v>2117</v>
       </c>
       <c r="B24">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A25" t="s">
         <v>2118</v>
       </c>
       <c r="B25">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A26" t="s">
         <v>2119</v>
       </c>
       <c r="B26">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A27" t="s">
         <v>2120</v>
       </c>
       <c r="B27">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A28" t="s">
         <v>2121</v>
       </c>
       <c r="B28">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A29" t="s">
         <v>2122</v>
       </c>
       <c r="B29">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A30" t="s">
         <v>2123</v>
       </c>
       <c r="B30">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A31" t="s">
         <v>2124</v>
       </c>
       <c r="B31">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A32" t="s">
         <v>2125</v>
       </c>
       <c r="B32">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A33" t="s">
         <v>2126</v>
       </c>
       <c r="B33">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>329</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A34" t="s">
         <v>2127</v>
       </c>
       <c r="B34">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A35" t="s">
         <v>2128</v>
       </c>
       <c r="B35">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A36" t="s">
         <v>2129</v>
       </c>
       <c r="B36">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A37" t="s">
         <v>2130</v>
       </c>
       <c r="B37">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A38" t="s">
         <v>2131</v>
       </c>
       <c r="B38">
         <v>1.87</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A39" t="s">
         <v>2132</v>
       </c>
       <c r="B39">
         <v>2.5499999999999998</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A40" t="s">
         <v>2133</v>
       </c>
       <c r="B40">
         <v>4.4800000000000004</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A41" t="s">
         <v>2134</v>
       </c>
       <c r="B41">
         <v>4.16</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A42" t="s">
         <v>2135</v>
       </c>
       <c r="B42">
         <v>3.83</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>424</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A43" t="s">
         <v>2136</v>
       </c>
       <c r="B43">
         <v>3.54</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A44" t="s">
         <v>2137</v>
       </c>
       <c r="B44">
         <v>4.45</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>446</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A45" t="s">
         <v>2138</v>
       </c>
       <c r="B45">
         <v>4.1900000000000004</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>457</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A46" t="s">
         <v>2139</v>
       </c>
       <c r="B46">
         <v>3.87</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>467</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A47" t="s">
         <v>2140</v>
       </c>
       <c r="B47">
         <v>3.58</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>477</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A48" t="s">
         <v>2141</v>
       </c>
       <c r="B48">
         <v>3.33</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>489</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A49" t="s">
         <v>2142</v>
       </c>
       <c r="B49">
         <v>3.12</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A50" t="s">
         <v>2143</v>
       </c>
       <c r="B50">
         <v>2.93</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>509</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A51" t="s">
         <v>2144</v>
       </c>
       <c r="B51">
         <v>2.76</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A52" t="s">
         <v>2145</v>
       </c>
       <c r="B52">
         <v>2.88</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A53" t="s">
         <v>2146</v>
       </c>
       <c r="B53">
         <v>2.71</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>542</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A54" t="s">
         <v>2147</v>
       </c>
       <c r="B54">
         <v>2.57</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>552</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A55" t="s">
         <v>2148</v>
       </c>
       <c r="B55">
         <v>2.4300000000000002</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>562</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A56" t="s">
         <v>2149</v>
       </c>
       <c r="B56">
         <v>2.3199999999999998</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>574</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A57" t="s">
         <v>2150</v>
       </c>
       <c r="B57">
         <v>2.21</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>584</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A58" t="s">
         <v>2151</v>
       </c>
       <c r="B58">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>594</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A59" t="s">
         <v>2152</v>
       </c>
       <c r="B59">
         <v>2.27</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>605</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A60" t="s">
         <v>2153</v>
       </c>
       <c r="B60">
         <v>2.16</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>615</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A61" t="s">
         <v>2154</v>
       </c>
       <c r="B61">
         <v>2.06</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A62" t="s">
         <v>2155</v>
       </c>
       <c r="B62">
         <v>3.09</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>637</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A63" t="s">
         <v>2156</v>
       </c>
       <c r="B63">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>647</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A64" t="s">
         <v>2157</v>
       </c>
       <c r="B64">
         <v>2.73</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>658</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A65" t="s">
         <v>2158</v>
       </c>
       <c r="B65">
         <v>3.52</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>669</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A66" t="s">
         <v>2159</v>
       </c>
       <c r="B66">
         <v>3.89</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>679</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A67" t="s">
         <v>2160</v>
       </c>
       <c r="B67">
         <v>3.89</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C67">
+        <f t="shared" ref="C67:C130" si="1">RIGHT(A67,4)-RIGHT($A$2,4)</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A68" t="s">
         <v>2161</v>
       </c>
       <c r="B68">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A69" t="s">
         <v>2162</v>
       </c>
       <c r="B69">
         <v>3.34</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>712</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A70" t="s">
         <v>2163</v>
       </c>
       <c r="B70">
         <v>3.12</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>722</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A71" t="s">
         <v>2164</v>
       </c>
       <c r="B71">
         <v>4.2300000000000004</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>732</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A72" t="s">
         <v>2165</v>
       </c>
       <c r="B72">
         <v>3.88</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>743</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A73" t="s">
         <v>2166</v>
       </c>
       <c r="B73">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>754</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A74" t="s">
         <v>2167</v>
       </c>
       <c r="B74">
         <v>3.34</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>764</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A75" t="s">
         <v>2168</v>
       </c>
       <c r="B75">
         <v>3.13</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A76" t="s">
         <v>2169</v>
       </c>
       <c r="B76">
         <v>2.94</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>785</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A77" t="s">
         <v>2170</v>
       </c>
       <c r="B77">
         <v>2.77</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>797</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A78" t="s">
         <v>2171</v>
       </c>
       <c r="B78">
         <v>4.49</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>807</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A79" t="s">
         <v>2172</v>
       </c>
       <c r="B79">
         <v>4.09</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>817</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A80" t="s">
         <v>2173</v>
       </c>
       <c r="B80">
         <v>3.78</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>828</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A81" t="s">
         <v>2174</v>
       </c>
       <c r="B81">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>839</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A82" t="s">
         <v>2175</v>
       </c>
       <c r="B82">
         <v>3.26</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>849</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A83" t="s">
         <v>2176</v>
       </c>
       <c r="B83">
         <v>3.06</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>860</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A84" t="s">
         <v>2177</v>
       </c>
       <c r="B84">
         <v>2.87</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>870</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A85" t="s">
         <v>2178</v>
       </c>
       <c r="B85">
         <v>2.72</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>882</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A86" t="s">
         <v>2179</v>
       </c>
       <c r="B86">
         <v>2.57</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>892</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A87" t="s">
         <v>2180</v>
       </c>
       <c r="B87">
         <v>2.46</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>902</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A88" t="s">
         <v>2181</v>
       </c>
       <c r="B88">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>913</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A89" t="s">
         <v>2182</v>
       </c>
       <c r="B89">
         <v>3.63</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C89">
+        <f t="shared" si="1"/>
+        <v>924</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A90" t="s">
         <v>2183</v>
       </c>
       <c r="B90">
         <v>4.47</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C90">
+        <f t="shared" si="1"/>
+        <v>934</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A91" t="s">
         <v>2184</v>
       </c>
       <c r="B91">
         <v>4.07</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C91">
+        <f t="shared" si="1"/>
+        <v>945</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A92" t="s">
         <v>2185</v>
       </c>
       <c r="B92">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C92">
+        <f t="shared" si="1"/>
+        <v>955</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A93" t="s">
         <v>2186</v>
       </c>
       <c r="B93">
         <v>3.48</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C93">
+        <f t="shared" si="1"/>
+        <v>967</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A94" t="s">
         <v>2187</v>
       </c>
       <c r="B94">
         <v>4</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>977</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A95" t="s">
         <v>2188</v>
       </c>
       <c r="B95">
         <v>3.69</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>987</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A96" t="s">
         <v>2189</v>
       </c>
       <c r="B96">
         <v>3.62</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A97" t="s">
         <v>2190</v>
       </c>
       <c r="B97">
         <v>3.87</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A98" t="s">
         <v>2191</v>
       </c>
       <c r="B98">
         <v>4.21</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A99" t="s">
         <v>2192</v>
       </c>
       <c r="B99">
         <v>3.87</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A100" t="s">
         <v>2193</v>
       </c>
       <c r="B100">
         <v>4.4800000000000004</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C100">
+        <f t="shared" si="1"/>
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A101" t="s">
         <v>2194</v>
       </c>
       <c r="B101">
         <v>4.4800000000000004</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A102" t="s">
         <v>2195</v>
       </c>
       <c r="B102">
         <v>4.4800000000000004</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C102">
+        <f t="shared" si="1"/>
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A103" t="s">
         <v>2196</v>
       </c>
       <c r="B103">
         <v>4.41</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C103">
+        <f t="shared" si="1"/>
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A104" t="s">
         <v>2197</v>
       </c>
       <c r="B104">
         <v>4.17</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C104">
+        <f t="shared" si="1"/>
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A105" t="s">
         <v>2198</v>
       </c>
       <c r="B105">
         <v>3.84</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C105">
+        <f t="shared" si="1"/>
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A106" t="s">
         <v>2199</v>
       </c>
       <c r="B106">
         <v>3.55</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C106">
+        <f t="shared" si="1"/>
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A107" t="s">
         <v>2200</v>
       </c>
       <c r="B107">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C107">
+        <f t="shared" si="1"/>
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A108" t="s">
         <v>2201</v>
       </c>
       <c r="B108">
         <v>4.09</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C108">
+        <f t="shared" si="1"/>
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A109" t="s">
         <v>2202</v>
       </c>
       <c r="B109">
         <v>3.77</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C109">
+        <f t="shared" si="1"/>
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A110" t="s">
         <v>2203</v>
       </c>
       <c r="B110">
         <v>3.49</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C110">
+        <f t="shared" si="1"/>
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A111" t="s">
         <v>2204</v>
       </c>
       <c r="B111">
         <v>3.26</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C111">
+        <f t="shared" si="1"/>
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A112" t="s">
         <v>2205</v>
       </c>
       <c r="B112">
         <v>3.91</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C112">
+        <f t="shared" si="1"/>
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A113" t="s">
         <v>2206</v>
       </c>
       <c r="B113">
         <v>3.72</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C113">
+        <f t="shared" si="1"/>
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A114" t="s">
         <v>2207</v>
       </c>
       <c r="B114">
         <v>3.73</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C114">
+        <f t="shared" si="1"/>
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A115" t="s">
         <v>2208</v>
       </c>
       <c r="B115">
         <v>3.47</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C115">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A116" t="s">
         <v>2209</v>
       </c>
       <c r="B116">
         <v>3.23</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C116">
+        <f t="shared" si="1"/>
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A117" t="s">
         <v>2210</v>
       </c>
       <c r="B117">
         <v>3.03</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C117">
+        <f t="shared" si="1"/>
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A118" t="s">
         <v>2211</v>
       </c>
       <c r="B118">
         <v>2.84</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C118">
+        <f t="shared" si="1"/>
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A119" t="s">
         <v>2212</v>
       </c>
       <c r="B119">
         <v>2.69</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C119">
+        <f t="shared" si="1"/>
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A120" t="s">
         <v>2213</v>
       </c>
       <c r="B120">
         <v>2.54</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C120">
+        <f t="shared" si="1"/>
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A121" t="s">
         <v>2214</v>
       </c>
       <c r="B121">
         <v>2.41</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C121">
+        <f t="shared" si="1"/>
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A122" t="s">
         <v>2215</v>
       </c>
       <c r="B122">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C122">
+        <f t="shared" si="1"/>
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A123" t="s">
         <v>2216</v>
       </c>
       <c r="B123">
         <v>2.19</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C123">
+        <f t="shared" si="1"/>
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A124" t="s">
         <v>2217</v>
       </c>
       <c r="B124">
         <v>2.09</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C124">
+        <f t="shared" si="1"/>
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A125" t="s">
         <v>2218</v>
       </c>
       <c r="B125">
         <v>2.17</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C125">
+        <f t="shared" si="1"/>
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A126" t="s">
         <v>2219</v>
       </c>
       <c r="B126">
         <v>2.06</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C126">
+        <f t="shared" si="1"/>
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A127" t="s">
         <v>2220</v>
       </c>
       <c r="B127">
         <v>1.97</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C127">
+        <f t="shared" si="1"/>
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A128" t="s">
         <v>2221</v>
       </c>
       <c r="B128">
         <v>1.89</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C128">
+        <f t="shared" si="1"/>
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A129" t="s">
         <v>2222</v>
       </c>
       <c r="B129">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C129">
+        <f t="shared" si="1"/>
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A130" t="s">
         <v>2223</v>
       </c>
       <c r="B130">
         <v>1.74</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C130">
+        <f t="shared" si="1"/>
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A131" t="s">
         <v>2224</v>
       </c>
       <c r="B131">
         <v>1.68</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C131">
+        <f t="shared" ref="C131:C194" si="2">RIGHT(A131,4)-RIGHT($A$2,4)</f>
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A132" t="s">
         <v>2225</v>
       </c>
       <c r="B132">
         <v>1.61</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C132">
+        <f t="shared" si="2"/>
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A133" t="s">
         <v>2226</v>
       </c>
       <c r="B133">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C133">
+        <f t="shared" si="2"/>
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A134" t="s">
         <v>2227</v>
       </c>
       <c r="B134">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C134">
+        <f t="shared" si="2"/>
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A135" t="s">
         <v>2228</v>
       </c>
       <c r="B135">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C135">
+        <f t="shared" si="2"/>
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A136" t="s">
         <v>2229</v>
       </c>
       <c r="B136">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C136">
+        <f t="shared" si="2"/>
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A137" t="s">
         <v>2230</v>
       </c>
       <c r="B137">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C137">
+        <f t="shared" si="2"/>
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A138" t="s">
         <v>2231</v>
       </c>
       <c r="B138">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C138">
+        <f t="shared" si="2"/>
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A139" t="s">
         <v>2232</v>
       </c>
       <c r="B139">
         <v>1.27</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C139">
+        <f t="shared" si="2"/>
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A140" t="s">
         <v>2233</v>
       </c>
       <c r="B140">
         <v>1.22</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C140">
+        <f t="shared" si="2"/>
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A141" t="s">
         <v>2234</v>
       </c>
       <c r="B141">
         <v>1.18</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C141">
+        <f t="shared" si="2"/>
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A142" t="s">
         <v>2235</v>
       </c>
       <c r="B142">
         <v>1.1499999999999999</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C142">
+        <f t="shared" si="2"/>
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A143" t="s">
         <v>2236</v>
       </c>
       <c r="B143">
         <v>1.1100000000000001</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C143">
+        <f t="shared" si="2"/>
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A144" t="s">
         <v>2237</v>
       </c>
       <c r="B144">
         <v>1.08</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C144">
+        <f t="shared" si="2"/>
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A145" t="s">
         <v>2238</v>
       </c>
       <c r="B145">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C145">
+        <f t="shared" si="2"/>
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A146" t="s">
         <v>2239</v>
       </c>
       <c r="B146">
         <v>1.02</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C146">
+        <f t="shared" si="2"/>
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A147" t="s">
         <v>2240</v>
       </c>
       <c r="B147">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C147">
+        <f t="shared" si="2"/>
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A148" t="s">
         <v>2241</v>
       </c>
       <c r="B148">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C148">
+        <f t="shared" si="2"/>
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A149" t="s">
         <v>2242</v>
       </c>
       <c r="B149">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C149">
+        <f t="shared" si="2"/>
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A150" t="s">
         <v>2243</v>
       </c>
       <c r="B150">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C150">
+        <f t="shared" si="2"/>
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A151" t="s">
         <v>2244</v>
       </c>
       <c r="B151">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C151">
+        <f t="shared" si="2"/>
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A152" t="s">
         <v>2245</v>
       </c>
       <c r="B152">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C152">
+        <f t="shared" si="2"/>
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A153" t="s">
         <v>2246</v>
       </c>
       <c r="B153">
         <v>0.83</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C153">
+        <f t="shared" si="2"/>
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A154" t="s">
         <v>2247</v>
       </c>
       <c r="B154">
         <v>1.72</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C154">
+        <f t="shared" si="2"/>
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A155" t="s">
         <v>2248</v>
       </c>
       <c r="B155">
         <v>1.64</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C155">
+        <f t="shared" si="2"/>
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A156" t="s">
         <v>2249</v>
       </c>
       <c r="B156">
         <v>1.57</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C156">
+        <f t="shared" si="2"/>
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A157" t="s">
         <v>2250</v>
       </c>
       <c r="B157">
         <v>1.51</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C157">
+        <f t="shared" si="2"/>
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A158" t="s">
         <v>2251</v>
       </c>
       <c r="B158">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C158">
+        <f t="shared" si="2"/>
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A159" t="s">
         <v>2252</v>
       </c>
       <c r="B159">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C159">
+        <f t="shared" si="2"/>
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A160" t="s">
         <v>2253</v>
       </c>
       <c r="B160">
         <v>1.34</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C160">
+        <f t="shared" si="2"/>
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A161" t="s">
         <v>2254</v>
       </c>
       <c r="B161">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C161">
+        <f t="shared" si="2"/>
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A162" t="s">
         <v>2255</v>
       </c>
       <c r="B162">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C162">
+        <f t="shared" si="2"/>
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A163" t="s">
         <v>2256</v>
       </c>
       <c r="B163">
         <v>1.21</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C163">
+        <f t="shared" si="2"/>
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A164" t="s">
         <v>2257</v>
       </c>
       <c r="B164">
         <v>1.17</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C164">
+        <f t="shared" si="2"/>
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A165" t="s">
         <v>2258</v>
       </c>
       <c r="B165">
         <v>1.1299999999999999</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C165">
+        <f t="shared" si="2"/>
+        <v>1731</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A166" t="s">
         <v>2259</v>
       </c>
       <c r="B166">
         <v>1.0900000000000001</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C166">
+        <f t="shared" si="2"/>
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A167" t="s">
         <v>2260</v>
       </c>
       <c r="B167">
         <v>1.06</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C167">
+        <f t="shared" si="2"/>
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A168" t="s">
         <v>2261</v>
       </c>
       <c r="B168">
         <v>1.02</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C168">
+        <f t="shared" si="2"/>
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A169" t="s">
         <v>2262</v>
       </c>
       <c r="B169">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C169">
+        <f t="shared" si="2"/>
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A170" t="s">
         <v>2263</v>
       </c>
       <c r="B170">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C170">
+        <f t="shared" si="2"/>
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A171" t="s">
         <v>2264</v>
       </c>
       <c r="B171">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C171">
+        <f t="shared" si="2"/>
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A172" t="s">
         <v>2265</v>
       </c>
       <c r="B172">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C172">
+        <f t="shared" si="2"/>
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A173" t="s">
         <v>2266</v>
       </c>
       <c r="B173">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C173">
+        <f t="shared" si="2"/>
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A174" t="s">
         <v>2267</v>
       </c>
       <c r="B174">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C174">
+        <f t="shared" si="2"/>
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A175" t="s">
         <v>2268</v>
       </c>
       <c r="B175">
         <v>0.83</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C175">
+        <f t="shared" si="2"/>
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A176" t="s">
         <v>2269</v>
       </c>
       <c r="B176">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C176">
+        <f t="shared" si="2"/>
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A177" t="s">
         <v>2270</v>
       </c>
       <c r="B177">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C177">
+        <f t="shared" si="2"/>
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A178" t="s">
         <v>2271</v>
       </c>
       <c r="B178">
         <v>0.76</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C178">
+        <f t="shared" si="2"/>
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A179" t="s">
         <v>2272</v>
       </c>
       <c r="B179">
         <v>0.74</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C179">
+        <f t="shared" si="2"/>
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A180" t="s">
         <v>2273</v>
       </c>
       <c r="B180">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C180">
+        <f t="shared" si="2"/>
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A181" t="s">
         <v>2274</v>
       </c>
       <c r="B181">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C181">
+        <f t="shared" si="2"/>
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A182" t="s">
         <v>2275</v>
       </c>
       <c r="B182">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C182">
+        <f t="shared" si="2"/>
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A183" t="s">
         <v>2276</v>
       </c>
       <c r="B183">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C183">
+        <f t="shared" si="2"/>
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A184" t="s">
         <v>2277</v>
       </c>
       <c r="B184">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C184">
+        <f t="shared" si="2"/>
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A185" t="s">
         <v>2278</v>
       </c>
       <c r="B185">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C185">
+        <f t="shared" si="2"/>
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A186" t="s">
         <v>2279</v>
       </c>
       <c r="B186">
         <v>0.61</v>
       </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C186">
+        <f t="shared" si="2"/>
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A187" t="s">
         <v>2280</v>
       </c>
       <c r="B187">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C187">
+        <f t="shared" si="2"/>
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A188" t="s">
         <v>2281</v>
       </c>
       <c r="B188">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C188">
+        <f t="shared" si="2"/>
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A189" t="s">
         <v>2282</v>
       </c>
       <c r="B189">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C189">
+        <f t="shared" si="2"/>
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A190" t="s">
         <v>2283</v>
       </c>
       <c r="B190">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C190">
+        <f t="shared" si="2"/>
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A191" t="s">
         <v>2284</v>
       </c>
       <c r="B191">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C191">
+        <f t="shared" si="2"/>
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A192" t="s">
         <v>2285</v>
       </c>
       <c r="B192">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C192">
+        <f t="shared" si="2"/>
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A193" t="s">
         <v>2286</v>
       </c>
       <c r="B193">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C193">
+        <f t="shared" si="2"/>
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A194" t="s">
         <v>2287</v>
       </c>
       <c r="B194">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C194">
+        <f t="shared" si="2"/>
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A195" t="s">
         <v>2288</v>
       </c>
       <c r="B195">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C195">
+        <f t="shared" ref="C195:C258" si="3">RIGHT(A195,4)-RIGHT($A$2,4)</f>
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A196" t="s">
         <v>2289</v>
       </c>
       <c r="B196">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C196">
+        <f t="shared" si="3"/>
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A197" t="s">
         <v>2290</v>
       </c>
       <c r="B197">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C197">
+        <f t="shared" si="3"/>
+        <v>2071</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A198" t="s">
         <v>2291</v>
       </c>
       <c r="B198">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C198">
+        <f t="shared" si="3"/>
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A199" t="s">
         <v>2292</v>
       </c>
       <c r="B199">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C199">
+        <f t="shared" si="3"/>
+        <v>2092</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A200" t="s">
         <v>2293</v>
       </c>
       <c r="B200">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C200">
+        <f t="shared" si="3"/>
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A201" t="s">
         <v>2294</v>
       </c>
       <c r="B201">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C201">
+        <f t="shared" si="3"/>
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A202" t="s">
         <v>2295</v>
       </c>
       <c r="B202">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C202">
+        <f t="shared" si="3"/>
+        <v>2124</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A203" t="s">
         <v>2296</v>
       </c>
       <c r="B203">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C203">
+        <f t="shared" si="3"/>
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A204" t="s">
         <v>2297</v>
       </c>
       <c r="B204">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C204">
+        <f t="shared" si="3"/>
+        <v>2145</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A205" t="s">
         <v>2298</v>
       </c>
       <c r="B205">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C205">
+        <f t="shared" si="3"/>
+        <v>2156</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A206" t="s">
         <v>2299</v>
       </c>
       <c r="B206">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C206">
+        <f t="shared" si="3"/>
+        <v>2166</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A207" t="s">
         <v>2300</v>
       </c>
       <c r="B207">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C207">
+        <f t="shared" si="3"/>
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A208" t="s">
         <v>2301</v>
       </c>
       <c r="B208">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C208">
+        <f t="shared" si="3"/>
+        <v>2187</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A209" t="s">
         <v>2302</v>
       </c>
       <c r="B209">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C209">
+        <f t="shared" si="3"/>
+        <v>2198</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A210" t="s">
         <v>2303</v>
       </c>
       <c r="B210">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C210">
+        <f t="shared" si="3"/>
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A211" t="s">
         <v>2304</v>
       </c>
       <c r="B211">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C211">
+        <f t="shared" si="3"/>
+        <v>2219</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A212" t="s">
         <v>2305</v>
       </c>
       <c r="B212">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C212">
+        <f t="shared" si="3"/>
+        <v>2230</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A213" t="s">
         <v>2306</v>
       </c>
       <c r="B213">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C213">
+        <f t="shared" si="3"/>
+        <v>2241</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A214" t="s">
         <v>2307</v>
       </c>
       <c r="B214">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C214">
+        <f t="shared" si="3"/>
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A215" t="s">
         <v>2308</v>
       </c>
       <c r="B215">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C215">
+        <f t="shared" si="3"/>
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A216" t="s">
         <v>2309</v>
       </c>
       <c r="B216">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C216">
+        <f t="shared" si="3"/>
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A217" t="s">
         <v>2310</v>
       </c>
       <c r="B217">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C217">
+        <f t="shared" si="3"/>
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A218" t="s">
         <v>2311</v>
       </c>
       <c r="B218">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C218">
+        <f t="shared" si="3"/>
+        <v>2294</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A219" t="s">
         <v>2312</v>
       </c>
       <c r="B219">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C219">
+        <f t="shared" si="3"/>
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A220" t="s">
         <v>2313</v>
       </c>
       <c r="B220">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C220">
+        <f t="shared" si="3"/>
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A221" t="s">
         <v>2314</v>
       </c>
       <c r="B221">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C221">
+        <f t="shared" si="3"/>
+        <v>2326</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A222" t="s">
         <v>2315</v>
       </c>
       <c r="B222">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C222">
+        <f t="shared" si="3"/>
+        <v>2336</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A223" t="s">
         <v>2316</v>
       </c>
       <c r="B223">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C223">
+        <f t="shared" si="3"/>
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A224" t="s">
         <v>2317</v>
       </c>
       <c r="B224">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C224">
+        <f t="shared" si="3"/>
+        <v>2357</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A225" t="s">
         <v>2318</v>
       </c>
       <c r="B225">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C225">
+        <f t="shared" si="3"/>
+        <v>2368</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A226" t="s">
         <v>2319</v>
       </c>
       <c r="B226">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C226">
+        <f t="shared" si="3"/>
+        <v>2379</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A227" t="s">
         <v>2320</v>
       </c>
       <c r="B227">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C227">
+        <f t="shared" si="3"/>
+        <v>2389</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A228" t="s">
         <v>2321</v>
       </c>
       <c r="B228">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C228">
+        <f t="shared" si="3"/>
+        <v>2399</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A229" t="s">
         <v>2322</v>
       </c>
       <c r="B229">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C229">
+        <f t="shared" si="3"/>
+        <v>2411</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A230" t="s">
         <v>2323</v>
       </c>
       <c r="B230">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C230">
+        <f t="shared" si="3"/>
+        <v>2421</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A231" t="s">
         <v>2324</v>
       </c>
       <c r="B231">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C231">
+        <f t="shared" si="3"/>
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A232" t="s">
         <v>2325</v>
       </c>
       <c r="B232">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C232">
+        <f t="shared" si="3"/>
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A233" t="s">
         <v>2326</v>
       </c>
       <c r="B233">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C233">
+        <f t="shared" si="3"/>
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A234" t="s">
         <v>2327</v>
       </c>
       <c r="B234">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C234">
+        <f t="shared" si="3"/>
+        <v>2464</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A235" t="s">
         <v>2328</v>
       </c>
       <c r="B235">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C235">
+        <f t="shared" si="3"/>
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A236" t="s">
         <v>2329</v>
       </c>
       <c r="B236">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C236">
+        <f t="shared" si="3"/>
+        <v>2484</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A237" t="s">
         <v>2330</v>
       </c>
       <c r="B237">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C237">
+        <f t="shared" si="3"/>
+        <v>2496</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A238" t="s">
         <v>2331</v>
       </c>
       <c r="B238">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C238">
+        <f t="shared" si="3"/>
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A239" t="s">
         <v>2332</v>
       </c>
       <c r="B239">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C239">
+        <f t="shared" si="3"/>
+        <v>2516</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A240" t="s">
         <v>2333</v>
       </c>
       <c r="B240">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C240">
+        <f t="shared" si="3"/>
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A241" t="s">
         <v>2334</v>
       </c>
       <c r="B241">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C241">
+        <f t="shared" si="3"/>
+        <v>2538</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A242" t="s">
         <v>2335</v>
       </c>
       <c r="B242">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C242">
+        <f t="shared" si="3"/>
+        <v>2549</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A243" t="s">
         <v>2336</v>
       </c>
       <c r="B243">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C243">
+        <f t="shared" si="3"/>
+        <v>2559</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A244" t="s">
         <v>2337</v>
       </c>
       <c r="B244">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C244">
+        <f t="shared" si="3"/>
+        <v>2569</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A245" t="s">
         <v>2338</v>
       </c>
       <c r="B245">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C245">
+        <f t="shared" si="3"/>
+        <v>2581</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A246" t="s">
         <v>2339</v>
       </c>
       <c r="B246">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C246">
+        <f t="shared" si="3"/>
+        <v>2591</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A247" t="s">
         <v>2340</v>
       </c>
       <c r="B247">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C247">
+        <f t="shared" si="3"/>
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A248" t="s">
         <v>2341</v>
       </c>
       <c r="B248">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C248">
+        <f t="shared" si="3"/>
+        <v>2612</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A249" t="s">
         <v>2342</v>
       </c>
       <c r="B249">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C249">
+        <f t="shared" si="3"/>
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A250" t="s">
         <v>2343</v>
       </c>
       <c r="B250">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C250">
+        <f t="shared" si="3"/>
+        <v>2634</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A251" t="s">
         <v>2344</v>
       </c>
       <c r="B251">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C251">
+        <f t="shared" si="3"/>
+        <v>2644</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A252" t="s">
         <v>2345</v>
       </c>
       <c r="B252">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C252">
+        <f t="shared" si="3"/>
+        <v>2654</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A253" t="s">
         <v>2346</v>
       </c>
       <c r="B253">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C253">
+        <f t="shared" si="3"/>
+        <v>2666</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A254" t="s">
         <v>2347</v>
       </c>
       <c r="B254">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C254">
+        <f t="shared" si="3"/>
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A255" t="s">
         <v>2348</v>
       </c>
       <c r="B255">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C255">
+        <f t="shared" si="3"/>
+        <v>2686</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A256" t="s">
         <v>2349</v>
       </c>
       <c r="B256">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C256">
+        <f t="shared" si="3"/>
+        <v>2697</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A257" t="s">
         <v>2350</v>
       </c>
       <c r="B257">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C257">
+        <f t="shared" si="3"/>
+        <v>2708</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A258" t="s">
         <v>2351</v>
       </c>
       <c r="B258">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C258">
+        <f t="shared" si="3"/>
+        <v>2718</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A259" t="s">
         <v>2352</v>
       </c>
       <c r="B259">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C259">
+        <f t="shared" ref="C259:C300" si="4">RIGHT(A259,4)-RIGHT($A$2,4)</f>
+        <v>2729</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A260" t="s">
         <v>2353</v>
       </c>
       <c r="B260">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C260">
+        <f t="shared" si="4"/>
+        <v>2739</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A261" t="s">
         <v>2354</v>
       </c>
       <c r="B261">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C261">
+        <f t="shared" si="4"/>
+        <v>2751</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A262" t="s">
         <v>2355</v>
       </c>
       <c r="B262">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C262">
+        <f t="shared" si="4"/>
+        <v>2761</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A263" t="s">
         <v>2356</v>
       </c>
       <c r="B263">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C263">
+        <f t="shared" si="4"/>
+        <v>2771</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A264" t="s">
         <v>2357</v>
       </c>
       <c r="B264">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C264">
+        <f t="shared" si="4"/>
+        <v>2782</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A265" t="s">
         <v>2358</v>
       </c>
       <c r="B265">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C265">
+        <f t="shared" si="4"/>
+        <v>2793</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A266" t="s">
         <v>2359</v>
       </c>
       <c r="B266">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C266">
+        <f t="shared" si="4"/>
+        <v>2803</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A267" t="s">
         <v>2360</v>
       </c>
       <c r="B267">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C267">
+        <f t="shared" si="4"/>
+        <v>2814</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A268" t="s">
         <v>2361</v>
       </c>
       <c r="B268">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C268">
+        <f t="shared" si="4"/>
+        <v>2824</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A269" t="s">
         <v>2362</v>
       </c>
       <c r="B269">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C269">
+        <f t="shared" si="4"/>
+        <v>2834</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A270" t="s">
         <v>2363</v>
       </c>
       <c r="B270">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C270">
+        <f t="shared" si="4"/>
+        <v>2846</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A271" t="s">
         <v>2364</v>
       </c>
       <c r="B271">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C271">
+        <f t="shared" si="4"/>
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A272" t="s">
         <v>2365</v>
       </c>
       <c r="B272">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C272">
+        <f t="shared" si="4"/>
+        <v>2866</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A273" t="s">
         <v>2366</v>
       </c>
       <c r="B273">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C273">
+        <f t="shared" si="4"/>
+        <v>2878</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A274" t="s">
         <v>2367</v>
       </c>
       <c r="B274">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C274">
+        <f t="shared" si="4"/>
+        <v>2888</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A275" t="s">
         <v>2368</v>
       </c>
       <c r="B275">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C275">
+        <f t="shared" si="4"/>
+        <v>2899</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A276" t="s">
         <v>2369</v>
       </c>
       <c r="B276">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C276">
+        <f t="shared" si="4"/>
+        <v>2909</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A277" t="s">
         <v>2370</v>
       </c>
       <c r="B277">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C277">
+        <f t="shared" si="4"/>
+        <v>2919</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A278" t="s">
         <v>2371</v>
       </c>
       <c r="B278">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C278">
+        <f t="shared" si="4"/>
+        <v>2931</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A279" t="s">
         <v>2372</v>
       </c>
       <c r="B279">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C279">
+        <f t="shared" si="4"/>
+        <v>2941</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A280" t="s">
         <v>2373</v>
       </c>
       <c r="B280">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C280">
+        <f t="shared" si="4"/>
+        <v>2951</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A281" t="s">
         <v>2374</v>
       </c>
       <c r="B281">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C281">
+        <f t="shared" si="4"/>
+        <v>2962</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A282" t="s">
         <v>2375</v>
       </c>
       <c r="B282">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C282">
+        <f t="shared" si="4"/>
+        <v>2973</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A283" t="s">
         <v>2376</v>
       </c>
       <c r="B283">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C283">
+        <f t="shared" si="4"/>
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A284" t="s">
         <v>2377</v>
       </c>
       <c r="B284">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C284">
+        <f t="shared" si="4"/>
+        <v>2994</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A285" t="s">
         <v>2378</v>
       </c>
       <c r="B285">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C285">
+        <f t="shared" si="4"/>
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A286" t="s">
         <v>2379</v>
       </c>
       <c r="B286">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C286">
+        <f t="shared" si="4"/>
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A287" t="s">
         <v>2380</v>
       </c>
       <c r="B287">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C287">
+        <f t="shared" si="4"/>
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A288" t="s">
         <v>2381</v>
       </c>
       <c r="B288">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C288">
+        <f t="shared" si="4"/>
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A289" t="s">
         <v>2382</v>
       </c>
       <c r="B289">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C289">
+        <f t="shared" si="4"/>
+        <v>3047</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A290" t="s">
         <v>2383</v>
       </c>
       <c r="B290">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C290">
+        <f t="shared" si="4"/>
+        <v>3058</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A291" t="s">
         <v>2384</v>
       </c>
       <c r="B291">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C291">
+        <f t="shared" si="4"/>
+        <v>3068</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A292" t="s">
         <v>2385</v>
       </c>
       <c r="B292">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C292">
+        <f t="shared" si="4"/>
+        <v>3079</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A293" t="s">
         <v>2386</v>
       </c>
       <c r="B293">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C293">
+        <f t="shared" si="4"/>
+        <v>3089</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A294" t="s">
         <v>2387</v>
       </c>
       <c r="B294">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C294">
+        <f t="shared" si="4"/>
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A295" t="s">
         <v>2388</v>
       </c>
       <c r="B295">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C295">
+        <f t="shared" si="4"/>
+        <v>3111</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A296" t="s">
         <v>2389</v>
       </c>
       <c r="B296">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C296">
+        <f t="shared" si="4"/>
+        <v>3121</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A297" t="s">
         <v>2390</v>
       </c>
       <c r="B297">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C297">
+        <f t="shared" si="4"/>
+        <v>3132</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A298" t="s">
         <v>2391</v>
       </c>
       <c r="B298">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C298">
+        <f t="shared" si="4"/>
+        <v>3143</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A299" t="s">
         <v>2392</v>
       </c>
       <c r="B299">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="C299">
+        <f t="shared" si="4"/>
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A300" t="s">
         <v>2393</v>
       </c>
       <c r="B300">
         <v>0.03</v>
+      </c>
+      <c r="C300">
+        <f t="shared" si="4"/>
+        <v>3164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>